<commit_message>
v0.0.13 updated to remove excess fluid prior to start
</commit_message>
<xml_diff>
--- a/Examples/CrystallisationTests/NeaveExperiments/Villiger2007_Petrolog_noOpx_Liq.xlsx
+++ b/Examples/CrystallisationTests/NeaveExperiments/Villiger2007_Petrolog_noOpx_Liq.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\2022\GitHub\pyMELTScalc\Examples\CrystallisationTests\NeaveExperiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\2022\GitHub\pyMELTScalc\Examples\CrystallisationTests\NeaveExperiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AC4BE53-374C-46A8-8441-99C0A8E7BC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC2B766-FE6A-4CB4-B7D4-31BB9FABBC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{896D3C4E-1DB1-45B0-8393-023EA2431F2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{896D3C4E-1DB1-45B0-8393-023EA2431F2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>SIO2_Liq</t>
-  </si>
   <si>
     <t>TiO2_Liq</t>
   </si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>FeOt_Liq</t>
+  </si>
+  <si>
+    <t>SiO2_Liq</t>
   </si>
 </sst>
 </file>
@@ -425,51 +425,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B26FA0-7026-4E27-979F-D26E151675BE}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>48.686999999999998</v>
       </c>
@@ -507,7 +505,7 @@
         <v>0.2001</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>48.7607</v>
       </c>
@@ -545,7 +543,7 @@
         <v>0.2021</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>48.837000000000003</v>
       </c>
@@ -583,7 +581,7 @@
         <v>0.20419999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>48.914499999999997</v>
       </c>
@@ -621,7 +619,7 @@
         <v>0.20630000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>48.994799999999998</v>
       </c>
@@ -659,7 +657,7 @@
         <v>0.2084</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>49.076300000000003</v>
       </c>
@@ -697,7 +695,7 @@
         <v>0.21060000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>49.160800000000002</v>
       </c>
@@ -735,7 +733,7 @@
         <v>0.21279999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>49.247500000000002</v>
       </c>
@@ -773,7 +771,7 @@
         <v>0.21510000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>49.336500000000001</v>
       </c>
@@ -811,7 +809,7 @@
         <v>0.2175</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>49.428699999999999</v>
       </c>
@@ -849,7 +847,7 @@
         <v>0.21990000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>49.504300000000001</v>
       </c>
@@ -887,7 +885,7 @@
         <v>0.22189999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>49.498800000000003</v>
       </c>
@@ -925,7 +923,7 @@
         <v>0.2223</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>49.468000000000004</v>
       </c>
@@ -963,7 +961,7 @@
         <v>0.2248</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>49.436999999999998</v>
       </c>
@@ -1001,7 +999,7 @@
         <v>0.22739999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>49.405700000000003</v>
       </c>
@@ -1039,7 +1037,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>49.374000000000002</v>
       </c>
@@ -1077,7 +1075,7 @@
         <v>0.23269999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>49.342100000000002</v>
       </c>
@@ -1115,7 +1113,7 @@
         <v>0.2354</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>49.31</v>
       </c>
@@ -1153,7 +1151,7 @@
         <v>0.2382</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>49.277500000000003</v>
       </c>
@@ -1191,7 +1189,7 @@
         <v>0.24110000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>49.244900000000001</v>
       </c>
@@ -1229,7 +1227,7 @@
         <v>0.24399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>49.211799999999997</v>
       </c>
@@ -1267,7 +1265,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>49.178600000000003</v>
       </c>
@@ -1305,7 +1303,7 @@
         <v>0.25009999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>49.145099999999999</v>
       </c>
@@ -1343,7 +1341,7 @@
         <v>0.25330000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>49.111499999999999</v>
       </c>
@@ -1381,7 +1379,7 @@
         <v>0.25650000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>49.077599999999997</v>
       </c>
@@ -1419,7 +1417,7 @@
         <v>0.25979999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>49.061999999999998</v>
       </c>
@@ -1457,7 +1455,7 @@
         <v>0.26140000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>49.053899999999999</v>
       </c>
@@ -1495,7 +1493,7 @@
         <v>0.26329999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>49.038200000000003</v>
       </c>
@@ -1533,7 +1531,7 @@
         <v>0.26679999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>49.036099999999998</v>
       </c>
@@ -1571,7 +1569,7 @@
         <v>0.27039999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>49.036299999999997</v>
       </c>
@@ -1609,7 +1607,7 @@
         <v>0.27410000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>49.036099999999998</v>
       </c>
@@ -1647,7 +1645,7 @@
         <v>0.27789999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>49.035800000000002</v>
       </c>
@@ -1685,7 +1683,7 @@
         <v>0.28179999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>49.034599999999998</v>
       </c>
@@ -1723,7 +1721,7 @@
         <v>0.2858</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>49.034199999999998</v>
       </c>
@@ -1761,7 +1759,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>49.033499999999997</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>0.29420000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>49.031999999999996</v>
       </c>
@@ -1837,7 +1835,7 @@
         <v>0.29859999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>49.03</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>0.30309999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>49.027500000000003</v>
       </c>
@@ -1913,7 +1911,7 @@
         <v>0.30780000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>49.025599999999997</v>
       </c>
@@ -1951,7 +1949,7 @@
         <v>0.31259999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>49.021999999999998</v>
       </c>
@@ -1989,7 +1987,7 @@
         <v>0.31759999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>49.018700000000003</v>
       </c>
@@ -2027,7 +2025,7 @@
         <v>0.32269999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>49.015099999999997</v>
       </c>
@@ -2065,7 +2063,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>49.011699999999998</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>0.33350000000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>49.006500000000003</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>0.33910000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>49.0017</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>0.34489999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>48.996099999999998</v>
       </c>
@@ -2217,7 +2215,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>48.989699999999999</v>
       </c>
@@ -2255,7 +2253,7 @@
         <v>0.35730000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48.983400000000003</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>0.36380000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48.976399999999998</v>
       </c>
@@ -2331,7 +2329,7 @@
         <v>0.3705</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48.968200000000003</v>
       </c>
@@ -2369,7 +2367,7 @@
         <v>0.3775</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>48.959200000000003</v>
       </c>
@@ -2407,7 +2405,7 @@
         <v>0.38469999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>48.950200000000002</v>
       </c>
@@ -2445,7 +2443,7 @@
         <v>0.39229999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>48.94</v>
       </c>
@@ -2483,7 +2481,7 @@
         <v>0.4002</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>48.928699999999999</v>
       </c>
@@ -2521,7 +2519,7 @@
         <v>0.4083</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>48.917299999999997</v>
       </c>
@@ -2559,7 +2557,7 @@
         <v>0.4168</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>48.903399999999998</v>
       </c>
@@ -2597,7 +2595,7 @@
         <v>0.42570000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>48.890500000000003</v>
       </c>
@@ -2635,7 +2633,7 @@
         <v>0.43490000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>48.875900000000001</v>
       </c>
@@ -2673,7 +2671,7 @@
         <v>0.4446</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>48.858699999999999</v>
       </c>
@@ -2711,7 +2709,7 @@
         <v>0.45469999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>48.842100000000002</v>
       </c>
@@ -2749,7 +2747,7 @@
         <v>0.46529999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>48.823900000000002</v>
       </c>
@@ -2787,7 +2785,7 @@
         <v>0.47639999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>48.803699999999999</v>
       </c>
@@ -2825,7 +2823,7 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>48.782600000000002</v>
       </c>
@@ -2863,7 +2861,7 @@
         <v>0.50019999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>48.759599999999999</v>
       </c>
@@ -2901,7 +2899,7 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>48.735300000000002</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>0.52649999999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>48.7087</v>
       </c>
@@ -2977,7 +2975,7 @@
         <v>0.54079999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>48.680700000000002</v>
       </c>
@@ -3015,7 +3013,7 @@
         <v>0.55579999999999996</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>48.650199999999998</v>
       </c>
@@ -3053,7 +3051,7 @@
         <v>0.5716</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>48.617699999999999</v>
       </c>
@@ -3091,7 +3089,7 @@
         <v>0.58850000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>48.583300000000001</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>0.60629999999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>48.5471</v>
       </c>
@@ -3167,7 +3165,7 @@
         <v>0.62519999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>48.506999999999998</v>
       </c>
@@ -3205,7 +3203,7 @@
         <v>0.64539999999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>48.464399999999998</v>
       </c>
@@ -3243,7 +3241,7 @@
         <v>0.66690000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>48.418999999999997</v>
       </c>
@@ -3281,7 +3279,7 @@
         <v>0.68989999999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>48.370399999999997</v>
       </c>
@@ -3319,7 +3317,7 @@
         <v>0.71460000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>48.3185</v>
       </c>
@@ -3357,7 +3355,7 @@
         <v>0.74099999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>48.2639</v>
       </c>
@@ -3395,7 +3393,7 @@
         <v>0.76959999999999995</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>48.204099999999997</v>
       </c>
@@ -3433,7 +3431,7 @@
         <v>0.80030000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>48.141100000000002</v>
       </c>
@@ -3471,7 +3469,7 @@
         <v>0.8337</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>48.074399999999997</v>
       </c>
@@ -3509,7 +3507,7 @@
         <v>0.86990000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>48.002699999999997</v>
       </c>
@@ -3547,7 +3545,7 @@
         <v>0.90939999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>47.929699999999997</v>
       </c>
@@ -3585,7 +3583,7 @@
         <v>0.95140000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>47.941499999999998</v>
       </c>
@@ -3623,7 +3621,7 @@
         <v>0.95269999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>48.383800000000001</v>
       </c>
@@ -3661,7 +3659,7 @@
         <v>1.0004</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>48.868899999999996</v>
       </c>
@@ -3699,7 +3697,7 @@
         <v>1.0529999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>49.4026</v>
       </c>
@@ -3737,7 +3735,7 @@
         <v>1.1114999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>49.992400000000004</v>
       </c>
@@ -3775,7 +3773,7 @@
         <v>1.1769000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>50.647300000000001</v>
       </c>
@@ -3813,7 +3811,7 @@
         <v>1.2504999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>51.380099999999999</v>
       </c>
@@ -3851,7 +3849,7 @@
         <v>1.3338000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>52.206000000000003</v>
       </c>
@@ -3889,7 +3887,7 @@
         <v>1.4291</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>53.162300000000002</v>
       </c>
@@ -3927,7 +3925,7 @@
         <v>1.5389999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>54.314700000000002</v>
       </c>
@@ -3965,7 +3963,7 @@
         <v>1.6674</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>55.685600000000001</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>1.8188</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>57.342100000000002</v>
       </c>
@@ -4041,7 +4039,7 @@
         <v>2.0007000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>59.383600000000001</v>
       </c>
@@ -4079,7 +4077,7 @@
         <v>2.2231000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>61.175899999999999</v>
       </c>

</xml_diff>